<commit_message>
Got rid of (most) overflows, added option to run forever.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0x88</t>
+          <t>0x63d4e7e</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -482,11 +482,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0x63d4e7e</t>
+          <t>0x55</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
@@ -503,11 +503,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0x55</t>
+          <t>0xe1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>524</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5">
@@ -524,11 +524,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0xe1</t>
+          <t>0xf1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>113</v>
+        <v>425</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,11 +545,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0xf1</t>
+          <t>0x101</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>552</v>
+        <v>10</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -566,11 +566,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0x101</t>
+          <t>0x8c</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -587,19 +587,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0x8c</t>
+          <t>0x111</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0x72</t>
+          <t>0xd0</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -608,19 +608,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0x111</t>
+          <t>0x151</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0x73</t>
+          <t>0xd1</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -629,19 +629,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0x151</t>
+          <t>0x1c</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0xa0</t>
+          <t>0xd2</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
@@ -650,7 +650,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0x1c</t>
+          <t>0x121</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -658,11 +658,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0xd0</t>
+          <t>0xd3</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -671,19 +671,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0x80</t>
+          <t>0xa8</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0xd1</t>
+          <t>0xd4</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
@@ -692,19 +692,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0x81</t>
+          <t>0xb0</t>
         </is>
       </c>
       <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0x170</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0xd2</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -713,15 +713,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0x121</t>
+          <t>0xb1</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0xd3</t>
+          <t>0x202</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -734,19 +734,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0x128</t>
+          <t>0xcc</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0xd4</t>
+          <t>0x203</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -755,19 +755,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0x140</t>
+          <t>0xcd</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0xbd</t>
+          <t>0x205</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
@@ -776,19 +776,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0x1d0</t>
+          <t>0x128</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0xbe</t>
+          <t>0x220</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18">
@@ -797,19 +797,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0xa8</t>
+          <t>0x140</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0xbf</t>
+          <t>0x221</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19">
@@ -818,15 +818,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0xb0</t>
+          <t>0x1d0</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0x171</t>
+          <t>0x72</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -839,82 +839,64 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0xb1</t>
+          <t>0x2aa</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0xc0</t>
+          <t>0x73</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>0xcc</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>4</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0x59</t>
+          <t>0xa0</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>0xcd</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>4</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0x211</t>
+          <t>0xa1</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>0x2aa</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>10</v>
-      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0xa1</t>
+          <t>0xa2</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -925,11 +907,11 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0x37</t>
+          <t>0xa3</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -940,11 +922,11 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0x9b</t>
+          <t>0xa4</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -955,11 +937,11 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0x3b</t>
+          <t>0xa6</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -970,11 +952,11 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0x210</t>
+          <t>0xbc</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -985,11 +967,11 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x4a</t>
+          <t>0x2c0</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>190</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1000,10 +982,220 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0x205</t>
+          <t>0x2c1</t>
         </is>
       </c>
       <c r="E29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0x59</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x131</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0xbd</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0xbe</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0xbf</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0x171</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0xc0</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x9b</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x211</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x210</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x37</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x3b</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x4a</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0x30</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to modify handshake.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1554</v>
+        <v>1515</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>

</xml_diff>

<commit_message>
Some successful tests w/ Brose.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>BatteryID</t>
+          <t>KvaserID</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>BikeID</t>
+          <t>MicrochipID</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -461,19 +461,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0xf1</t>
+          <t>0x300</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1515</v>
+        <v>122</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0x9a</t>
+          <t>0x400</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>76</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
@@ -482,19 +482,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0x111</t>
+          <t>0x203</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0x72</t>
+          <t>0x401</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
@@ -503,19 +503,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0x80</t>
+          <t>0x202</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0x73</t>
+          <t>0x402</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -524,19 +524,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0x81</t>
+          <t>0x666</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0xc0</t>
+          <t>0x403</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -545,74 +545,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0x121</t>
+          <t>0x200</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0x128</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>33</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0xa8</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>34</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0xb0</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>34</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0xb1</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>34</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>